<commit_message>
Save before you commit, you idiot -.-
</commit_message>
<xml_diff>
--- a/Design/Assets.xlsx
+++ b/Design/Assets.xlsx
@@ -11,13 +11,147 @@
     <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
     <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="124519"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="43">
+  <si>
+    <t>Nr</t>
+  </si>
+  <si>
+    <t>Nazwa</t>
+  </si>
+  <si>
+    <t>Modele</t>
+  </si>
+  <si>
+    <t>Ściana_prosta</t>
+  </si>
+  <si>
+    <t>Ściana_prosta_wnęka</t>
+  </si>
+  <si>
+    <t>Ściana_róg_lewy</t>
+  </si>
+  <si>
+    <t>Ściana_róg_prawy</t>
+  </si>
+  <si>
+    <t>Ściana_prosta_drzwi</t>
+  </si>
+  <si>
+    <t>Sufit_prosty</t>
+  </si>
+  <si>
+    <t>Sufit_prosty_wnęka</t>
+  </si>
+  <si>
+    <t>Sufit_skos</t>
+  </si>
+  <si>
+    <t>Sufit_wypukły</t>
+  </si>
+  <si>
+    <t>Podłoga_prosta</t>
+  </si>
+  <si>
+    <t>Podłoga_stopień_niski</t>
+  </si>
+  <si>
+    <t>Podłoga_stopień_wysoki</t>
+  </si>
+  <si>
+    <t>Schody_1</t>
+  </si>
+  <si>
+    <t>Schody_2</t>
+  </si>
+  <si>
+    <t>Ilość wariantów kolorystycznych</t>
+  </si>
+  <si>
+    <t>Tiling</t>
+  </si>
+  <si>
+    <t>Poziomo</t>
+  </si>
+  <si>
+    <t>Poziomo / pionowo</t>
+  </si>
+  <si>
+    <t>Brak</t>
+  </si>
+  <si>
+    <t>Kolumna_1_trzon</t>
+  </si>
+  <si>
+    <t>Kolumna_1_głowica</t>
+  </si>
+  <si>
+    <t>Kolumna_1_baza</t>
+  </si>
+  <si>
+    <t>Kolumna_róg_lewy</t>
+  </si>
+  <si>
+    <t>Kolumna_róg_prawy</t>
+  </si>
+  <si>
+    <t>Drzwi</t>
+  </si>
+  <si>
+    <t>Poziomo (tworzy zakończenie ściany)</t>
+  </si>
+  <si>
+    <t>Kolumna_niska</t>
+  </si>
+  <si>
+    <t>Palenisko</t>
+  </si>
+  <si>
+    <t>Lampa</t>
+  </si>
+  <si>
+    <t>Wazon</t>
+  </si>
+  <si>
+    <t>Ławka</t>
+  </si>
+  <si>
+    <t>Posąg_1</t>
+  </si>
+  <si>
+    <t>Posąg_2</t>
+  </si>
+  <si>
+    <t>Tekstury</t>
+  </si>
+  <si>
+    <t>Podłoga_wzory</t>
+  </si>
+  <si>
+    <t>Podłoga_baza</t>
+  </si>
+  <si>
+    <t>Kolumna_1_wzory</t>
+  </si>
+  <si>
+    <t>Ściana_normalna</t>
+  </si>
+  <si>
+    <t>Ściana_wysoka</t>
+  </si>
+  <si>
+    <t>Ściana_wnęka</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -26,13 +160,34 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -47,8 +202,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -343,14 +503,616 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B56" sqref="B56"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="4.28515625" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="2" customFormat="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="1" customFormat="1">
+      <c r="A31" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35">
+        <v>4</v>
+      </c>
+      <c r="B35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36">
+        <v>5</v>
+      </c>
+      <c r="B36" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37">
+        <v>6</v>
+      </c>
+      <c r="B37" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38">
+        <v>7</v>
+      </c>
+      <c r="B38" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39">
+        <v>8</v>
+      </c>
+      <c r="B39" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40">
+        <v>9</v>
+      </c>
+      <c r="B40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41">
+        <v>10</v>
+      </c>
+      <c r="B41" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42">
+        <v>11</v>
+      </c>
+      <c r="B42" t="s">
+        <v>32</v>
+      </c>
+      <c r="C42" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43">
+        <v>12</v>
+      </c>
+      <c r="B43" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" t="s">
+        <v>21</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44">
+        <v>13</v>
+      </c>
+      <c r="B44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A31:C31"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Update with assets list + atlas
</commit_message>
<xml_diff>
--- a/Design/Assets.xlsx
+++ b/Design/Assets.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="56">
   <si>
     <t>Nr</t>
   </si>
@@ -75,12 +75,6 @@
     <t>Tiling</t>
   </si>
   <si>
-    <t>Poziomo</t>
-  </si>
-  <si>
-    <t>Poziomo / pionowo</t>
-  </si>
-  <si>
     <t>Brak</t>
   </si>
   <si>
@@ -102,9 +96,6 @@
     <t>Drzwi</t>
   </si>
   <si>
-    <t>Poziomo (tworzy zakończenie ściany)</t>
-  </si>
-  <si>
     <t>Kolumna_niska</t>
   </si>
   <si>
@@ -129,28 +120,80 @@
     <t>Tekstury</t>
   </si>
   <si>
-    <t>Podłoga_wzory</t>
-  </si>
-  <si>
-    <t>Podłoga_baza</t>
-  </si>
-  <si>
     <t>Kolumna_1_wzory</t>
   </si>
   <si>
-    <t>Ściana_normalna</t>
-  </si>
-  <si>
-    <t>Ściana_wysoka</t>
-  </si>
-  <si>
-    <t>Ściana_wnęka</t>
+    <t>Długość</t>
+  </si>
+  <si>
+    <t>Szerokość</t>
+  </si>
+  <si>
+    <t>Wysokość</t>
+  </si>
+  <si>
+    <t>Podłoga_1</t>
+  </si>
+  <si>
+    <t>Podłoga_4</t>
+  </si>
+  <si>
+    <t>1 kierunek</t>
+  </si>
+  <si>
+    <t>2 kierunek</t>
+  </si>
+  <si>
+    <t>2 kierunki</t>
+  </si>
+  <si>
+    <t>1 kierunek (tworzy zakończenie ściany)</t>
+  </si>
+  <si>
+    <t>Podłoga_2 + 3 + 5</t>
+  </si>
+  <si>
+    <t>Nr atlasu</t>
+  </si>
+  <si>
+    <t>Ściana_1</t>
+  </si>
+  <si>
+    <t>Ściana_2</t>
+  </si>
+  <si>
+    <t>Ściana_3</t>
+  </si>
+  <si>
+    <t>Ściana_4-1</t>
+  </si>
+  <si>
+    <t>Ściana_4-2</t>
+  </si>
+  <si>
+    <t>Sufit + drzwi</t>
+  </si>
+  <si>
+    <t>Atlas 1</t>
+  </si>
+  <si>
+    <t>Atlas 2</t>
+  </si>
+  <si>
+    <t>Atlas 3</t>
+  </si>
+  <si>
+    <t>Atlas 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.00&quot; m&quot;"/>
+    <numFmt numFmtId="165" formatCode="0.00&quot; px&quot;"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -190,7 +233,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -198,16 +241,485 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -503,22 +1015,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:Z253"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P38" sqref="P38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
     <col min="2" max="2" width="39.85546875" customWidth="1"/>
-    <col min="3" max="3" width="33.7109375" customWidth="1"/>
+    <col min="3" max="3" width="35.140625" customWidth="1"/>
     <col min="4" max="4" width="30.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" customWidth="1"/>
+    <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
+    <col min="11" max="26" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1">
+    <row r="1" spans="1:7" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -531,15 +1049,24 @@
       <c r="D1" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" s="1" customFormat="1">
-      <c r="A2" s="3" t="s">
+      <c r="E1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1">
+      <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>1</v>
       </c>
@@ -547,13 +1074,22 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="3">
+        <v>4</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G3" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>2</v>
       </c>
@@ -561,13 +1097,22 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="3">
+        <v>4</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>3</v>
       </c>
@@ -575,13 +1120,22 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="3">
+        <v>4</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>4</v>
       </c>
@@ -589,13 +1143,22 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" s="3">
+        <v>4</v>
+      </c>
+      <c r="F6" s="3">
+        <v>4</v>
+      </c>
+      <c r="G6" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>5</v>
       </c>
@@ -603,13 +1166,22 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" s="3">
+        <v>4</v>
+      </c>
+      <c r="F7" s="3">
+        <v>4</v>
+      </c>
+      <c r="G7" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>6</v>
       </c>
@@ -617,13 +1189,22 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" s="3">
+        <v>4</v>
+      </c>
+      <c r="F8" s="3">
+        <v>4</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>7</v>
       </c>
@@ -631,13 +1212,22 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" s="3">
+        <v>4</v>
+      </c>
+      <c r="F9" s="3">
+        <v>4</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>8</v>
       </c>
@@ -645,13 +1235,22 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" s="3">
+        <v>4</v>
+      </c>
+      <c r="F10" s="3">
+        <v>2</v>
+      </c>
+      <c r="G10" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>9</v>
       </c>
@@ -659,13 +1258,22 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" s="3">
+        <v>4</v>
+      </c>
+      <c r="F11" s="3">
+        <v>4</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>10</v>
       </c>
@@ -673,13 +1281,22 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" s="3">
+        <v>4</v>
+      </c>
+      <c r="F12" s="3">
+        <v>4</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>11</v>
       </c>
@@ -687,13 +1304,22 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13" s="3">
+        <v>4</v>
+      </c>
+      <c r="F13" s="3">
+        <v>4</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>12</v>
       </c>
@@ -701,13 +1327,22 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14" s="3">
+        <v>4</v>
+      </c>
+      <c r="F14" s="3">
+        <v>4</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>13</v>
       </c>
@@ -715,13 +1350,16 @@
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>14</v>
       </c>
@@ -729,202 +1367,255 @@
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:26">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:26">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:26">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:26">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:26">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:26">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:26">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="1:26">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:26">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:26">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:26">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="1:26">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+    </row>
+    <row r="29" spans="1:26">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C29" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" s="1" customFormat="1">
-      <c r="A31" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+    </row>
+    <row r="30" spans="1:26">
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+    </row>
+    <row r="31" spans="1:26" s="1" customFormat="1">
+      <c r="A31" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" ht="15.75" thickBot="1">
       <c r="A32">
         <v>1</v>
       </c>
@@ -932,184 +1623,1871 @@
         <v>38</v>
       </c>
       <c r="C32" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="D32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+        <v>1</v>
+      </c>
+      <c r="F32" s="5">
+        <v>1024</v>
+      </c>
+      <c r="G32" s="5">
+        <v>1024</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <f>F32*G32</f>
+        <v>1048576</v>
+      </c>
+      <c r="J32">
+        <v>1</v>
+      </c>
+      <c r="K32" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="10"/>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="10"/>
+      <c r="R32" s="10"/>
+      <c r="S32" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="T32" s="10"/>
+      <c r="U32" s="10"/>
+      <c r="V32" s="10"/>
+      <c r="W32" s="10"/>
+      <c r="X32" s="10"/>
+      <c r="Y32" s="10"/>
+      <c r="Z32" s="10"/>
+    </row>
+    <row r="33" spans="1:26" ht="15.75" thickTop="1">
       <c r="A33">
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C33" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="D33">
+        <v>3</v>
+      </c>
+      <c r="F33" s="5">
+        <v>512</v>
+      </c>
+      <c r="G33" s="5">
+        <v>512</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <f t="shared" ref="I33:I48" si="0">F33*G33</f>
+        <v>262144</v>
+      </c>
+      <c r="J33">
+        <v>2</v>
+      </c>
+      <c r="K33" s="12">
+        <v>1</v>
+      </c>
+      <c r="L33" s="13"/>
+      <c r="M33" s="14">
+        <v>2</v>
+      </c>
+      <c r="N33" s="14">
+        <v>6</v>
+      </c>
+      <c r="O33" s="15">
+        <v>4</v>
+      </c>
+      <c r="P33" s="15">
         <v>5</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="Q33" s="14">
+        <v>7</v>
+      </c>
+      <c r="R33" s="16">
+        <v>15</v>
+      </c>
+      <c r="S33" s="17"/>
+      <c r="T33" s="14"/>
+      <c r="U33" s="14"/>
+      <c r="V33" s="14"/>
+      <c r="W33" s="14"/>
+      <c r="X33" s="14"/>
+      <c r="Y33" s="14"/>
+      <c r="Z33" s="16"/>
+    </row>
+    <row r="34" spans="1:26">
       <c r="A34">
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="C34" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="F34" s="5">
+        <v>1024</v>
+      </c>
+      <c r="G34" s="5">
+        <v>512</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="0"/>
+        <v>524288</v>
+      </c>
+      <c r="J34">
+        <v>3</v>
+      </c>
+      <c r="K34" s="18"/>
+      <c r="L34" s="19"/>
+      <c r="M34" s="20">
+        <v>3</v>
+      </c>
+      <c r="N34" s="21"/>
+      <c r="O34" s="22"/>
+      <c r="P34" s="22"/>
+      <c r="Q34" s="23"/>
+      <c r="R34" s="24"/>
+      <c r="S34" s="25"/>
+      <c r="T34" s="23"/>
+      <c r="U34" s="23"/>
+      <c r="V34" s="23"/>
+      <c r="W34" s="23"/>
+      <c r="X34" s="23"/>
+      <c r="Y34" s="23"/>
+      <c r="Z34" s="24"/>
+    </row>
+    <row r="35" spans="1:26">
       <c r="A35">
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="C35" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="F35" s="5">
+        <v>512</v>
+      </c>
+      <c r="G35" s="5">
+        <v>1024</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="0"/>
+        <v>524288</v>
+      </c>
+      <c r="J35">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="K35" s="26">
+        <v>8</v>
+      </c>
+      <c r="L35" s="27"/>
+      <c r="M35" s="28">
+        <v>13</v>
+      </c>
+      <c r="N35" s="29">
+        <v>14</v>
+      </c>
+      <c r="O35" s="27"/>
+      <c r="P35" s="23"/>
+      <c r="Q35" s="23"/>
+      <c r="R35" s="24"/>
+      <c r="S35" s="25"/>
+      <c r="T35" s="23"/>
+      <c r="U35" s="23"/>
+      <c r="V35" s="23"/>
+      <c r="W35" s="23"/>
+      <c r="X35" s="23"/>
+      <c r="Y35" s="23"/>
+      <c r="Z35" s="24"/>
+    </row>
+    <row r="36" spans="1:26">
       <c r="A36">
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="D36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
+        <v>4</v>
+      </c>
+      <c r="F36" s="5">
+        <v>512</v>
+      </c>
+      <c r="G36" s="5">
+        <v>1024</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="0"/>
+        <v>524288</v>
+      </c>
+      <c r="J36">
+        <v>5</v>
+      </c>
+      <c r="K36" s="18"/>
+      <c r="L36" s="19"/>
+      <c r="M36" s="22"/>
+      <c r="N36" s="30"/>
+      <c r="O36" s="19"/>
+      <c r="P36" s="23"/>
+      <c r="Q36" s="23"/>
+      <c r="R36" s="24"/>
+      <c r="S36" s="25"/>
+      <c r="T36" s="23"/>
+      <c r="U36" s="23"/>
+      <c r="V36" s="23"/>
+      <c r="W36" s="23"/>
+      <c r="X36" s="23"/>
+      <c r="Y36" s="23"/>
+      <c r="Z36" s="24"/>
+    </row>
+    <row r="37" spans="1:26">
       <c r="A37">
         <v>6</v>
       </c>
       <c r="B37" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" t="s">
         <v>40</v>
       </c>
-      <c r="C37" t="s">
-        <v>19</v>
-      </c>
       <c r="D37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="F37" s="5">
+        <v>512</v>
+      </c>
+      <c r="G37" s="5">
+        <v>512</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="0"/>
+        <v>262144</v>
+      </c>
+      <c r="J37">
+        <v>6</v>
+      </c>
+      <c r="K37" s="26">
+        <v>9</v>
+      </c>
+      <c r="L37" s="27"/>
+      <c r="M37" s="28">
+        <v>10</v>
+      </c>
+      <c r="N37" s="23"/>
+      <c r="O37" s="23"/>
+      <c r="P37" s="23"/>
+      <c r="Q37" s="23"/>
+      <c r="R37" s="24"/>
+      <c r="S37" s="25"/>
+      <c r="T37" s="23"/>
+      <c r="U37" s="23"/>
+      <c r="V37" s="23"/>
+      <c r="W37" s="23"/>
+      <c r="X37" s="23"/>
+      <c r="Y37" s="23"/>
+      <c r="Z37" s="24"/>
+    </row>
+    <row r="38" spans="1:26">
       <c r="A38">
         <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C38" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="F38" s="5">
+        <v>512</v>
+      </c>
+      <c r="G38" s="5">
+        <v>512</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="0"/>
+        <v>262144</v>
+      </c>
+      <c r="J38">
+        <v>7</v>
+      </c>
+      <c r="K38" s="31"/>
+      <c r="L38" s="32"/>
+      <c r="M38" s="33"/>
+      <c r="N38" s="23"/>
+      <c r="O38" s="23"/>
+      <c r="P38" s="23"/>
+      <c r="Q38" s="23"/>
+      <c r="R38" s="24"/>
+      <c r="S38" s="25"/>
+      <c r="T38" s="23"/>
+      <c r="U38" s="23"/>
+      <c r="V38" s="23"/>
+      <c r="W38" s="23"/>
+      <c r="X38" s="23"/>
+      <c r="Y38" s="23"/>
+      <c r="Z38" s="24"/>
+    </row>
+    <row r="39" spans="1:26">
       <c r="A39">
         <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C39" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="F39" s="5">
+        <v>1024</v>
+      </c>
+      <c r="G39" s="5">
+        <v>1024</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="0"/>
+        <v>1048576</v>
+      </c>
+      <c r="J39">
+        <v>8</v>
+      </c>
+      <c r="K39" s="18"/>
+      <c r="L39" s="19"/>
+      <c r="M39" s="22"/>
+      <c r="N39" s="23"/>
+      <c r="O39" s="23"/>
+      <c r="P39" s="23"/>
+      <c r="Q39" s="23"/>
+      <c r="R39" s="24"/>
+      <c r="S39" s="25"/>
+      <c r="T39" s="23"/>
+      <c r="U39" s="23"/>
+      <c r="V39" s="23"/>
+      <c r="W39" s="23"/>
+      <c r="X39" s="23"/>
+      <c r="Y39" s="23"/>
+      <c r="Z39" s="24"/>
+    </row>
+    <row r="40" spans="1:26" ht="15.75" thickBot="1">
       <c r="A40">
         <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C40" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="F40" s="5">
+        <v>1024</v>
+      </c>
+      <c r="G40" s="5">
+        <v>1536</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="0"/>
+        <v>1572864</v>
+      </c>
+      <c r="J40">
+        <v>9</v>
+      </c>
+      <c r="K40" s="34">
+        <v>11</v>
+      </c>
+      <c r="L40" s="35">
+        <v>12</v>
+      </c>
+      <c r="M40" s="35"/>
+      <c r="N40" s="35"/>
+      <c r="O40" s="35"/>
+      <c r="P40" s="35"/>
+      <c r="Q40" s="35"/>
+      <c r="R40" s="36"/>
+      <c r="S40" s="34"/>
+      <c r="T40" s="35"/>
+      <c r="U40" s="35"/>
+      <c r="V40" s="35"/>
+      <c r="W40" s="35"/>
+      <c r="X40" s="35"/>
+      <c r="Y40" s="35"/>
+      <c r="Z40" s="36"/>
+    </row>
+    <row r="41" spans="1:26" ht="15.75" thickTop="1">
       <c r="A41">
         <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="C41" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="D41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="F41" s="5">
+        <v>512</v>
+      </c>
+      <c r="G41" s="5">
+        <v>1536</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="0"/>
+        <v>786432</v>
+      </c>
+      <c r="J41">
+        <v>10</v>
+      </c>
+      <c r="K41" s="37"/>
+      <c r="L41" s="38"/>
+      <c r="M41" s="38"/>
+      <c r="N41" s="38"/>
+      <c r="O41" s="38"/>
+      <c r="P41" s="38"/>
+      <c r="Q41" s="38"/>
+      <c r="R41" s="39"/>
+      <c r="S41" s="17"/>
+      <c r="T41" s="14"/>
+      <c r="U41" s="14"/>
+      <c r="V41" s="14"/>
+      <c r="W41" s="14"/>
+      <c r="X41" s="14"/>
+      <c r="Y41" s="14"/>
+      <c r="Z41" s="16"/>
+    </row>
+    <row r="42" spans="1:26">
       <c r="A42">
         <v>11</v>
       </c>
       <c r="B42" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="C42" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="D42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="F42" s="5">
+        <v>512</v>
+      </c>
+      <c r="G42" s="5">
+        <v>512</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="0"/>
+        <v>262144</v>
+      </c>
+      <c r="J42">
+        <v>11</v>
+      </c>
+      <c r="K42" s="25"/>
+      <c r="L42" s="23"/>
+      <c r="M42" s="23"/>
+      <c r="N42" s="23"/>
+      <c r="O42" s="23"/>
+      <c r="P42" s="23"/>
+      <c r="Q42" s="23"/>
+      <c r="R42" s="40"/>
+      <c r="S42" s="25"/>
+      <c r="T42" s="23"/>
+      <c r="U42" s="23"/>
+      <c r="V42" s="23"/>
+      <c r="W42" s="23"/>
+      <c r="X42" s="23"/>
+      <c r="Y42" s="23"/>
+      <c r="Z42" s="24"/>
+    </row>
+    <row r="43" spans="1:26">
       <c r="A43">
         <v>12</v>
       </c>
       <c r="B43" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="C43" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="D43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:4">
+      <c r="F43" s="5">
+        <v>512</v>
+      </c>
+      <c r="G43" s="5">
+        <v>512</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="0"/>
+        <v>262144</v>
+      </c>
+      <c r="J43">
+        <v>12</v>
+      </c>
+      <c r="K43" s="25"/>
+      <c r="L43" s="23"/>
+      <c r="M43" s="23"/>
+      <c r="N43" s="23"/>
+      <c r="O43" s="23"/>
+      <c r="P43" s="23"/>
+      <c r="Q43" s="23"/>
+      <c r="R43" s="40"/>
+      <c r="S43" s="25"/>
+      <c r="T43" s="23"/>
+      <c r="U43" s="23"/>
+      <c r="V43" s="23"/>
+      <c r="W43" s="23"/>
+      <c r="X43" s="23"/>
+      <c r="Y43" s="23"/>
+      <c r="Z43" s="24"/>
+    </row>
+    <row r="44" spans="1:26">
       <c r="A44">
         <v>13</v>
       </c>
       <c r="B44" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C44" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
+      <c r="F44" s="5">
+        <v>512</v>
+      </c>
+      <c r="G44" s="5">
+        <v>1024</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="0"/>
+        <v>524288</v>
+      </c>
+      <c r="J44">
+        <v>13</v>
+      </c>
+      <c r="K44" s="25"/>
+      <c r="L44" s="23"/>
+      <c r="M44" s="23"/>
+      <c r="N44" s="23"/>
+      <c r="O44" s="23"/>
+      <c r="P44" s="23"/>
+      <c r="Q44" s="23"/>
+      <c r="R44" s="40"/>
+      <c r="S44" s="25"/>
+      <c r="T44" s="23"/>
+      <c r="U44" s="23"/>
+      <c r="V44" s="23"/>
+      <c r="W44" s="23"/>
+      <c r="X44" s="23"/>
+      <c r="Y44" s="23"/>
+      <c r="Z44" s="24"/>
+    </row>
+    <row r="45" spans="1:26">
+      <c r="A45">
+        <v>14</v>
+      </c>
+      <c r="B45" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45" t="s">
+        <v>40</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="F45" s="5">
+        <v>1024</v>
+      </c>
+      <c r="G45" s="5">
+        <v>1024</v>
+      </c>
+      <c r="H45">
+        <v>1</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="0"/>
+        <v>1048576</v>
+      </c>
+      <c r="J45">
+        <v>14</v>
+      </c>
+      <c r="K45" s="25"/>
+      <c r="L45" s="23"/>
+      <c r="M45" s="23"/>
+      <c r="N45" s="23"/>
+      <c r="O45" s="23"/>
+      <c r="P45" s="23"/>
+      <c r="Q45" s="23"/>
+      <c r="R45" s="40"/>
+      <c r="S45" s="25"/>
+      <c r="T45" s="23"/>
+      <c r="U45" s="23"/>
+      <c r="V45" s="23"/>
+      <c r="W45" s="23"/>
+      <c r="X45" s="23"/>
+      <c r="Y45" s="23"/>
+      <c r="Z45" s="24"/>
+    </row>
+    <row r="46" spans="1:26">
+      <c r="A46">
+        <v>15</v>
+      </c>
+      <c r="B46" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" t="s">
+        <v>40</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="F46" s="5">
+        <v>512</v>
+      </c>
+      <c r="G46" s="5">
+        <v>512</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="0"/>
+        <v>262144</v>
+      </c>
+      <c r="J46">
+        <v>15</v>
+      </c>
+      <c r="K46" s="25"/>
+      <c r="L46" s="23"/>
+      <c r="M46" s="23"/>
+      <c r="N46" s="23"/>
+      <c r="O46" s="23"/>
+      <c r="P46" s="23"/>
+      <c r="Q46" s="23"/>
+      <c r="R46" s="40"/>
+      <c r="S46" s="25"/>
+      <c r="T46" s="23"/>
+      <c r="U46" s="23"/>
+      <c r="V46" s="23"/>
+      <c r="W46" s="23"/>
+      <c r="X46" s="23"/>
+      <c r="Y46" s="23"/>
+      <c r="Z46" s="24"/>
+    </row>
+    <row r="47" spans="1:26">
+      <c r="A47">
+        <v>16</v>
+      </c>
+      <c r="B47" t="s">
+        <v>31</v>
+      </c>
+      <c r="C47" t="s">
+        <v>19</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47">
+        <v>1</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>16</v>
+      </c>
+      <c r="K47" s="25"/>
+      <c r="L47" s="23"/>
+      <c r="M47" s="23"/>
+      <c r="N47" s="23"/>
+      <c r="O47" s="23"/>
+      <c r="P47" s="23"/>
+      <c r="Q47" s="23"/>
+      <c r="R47" s="40"/>
+      <c r="S47" s="25"/>
+      <c r="T47" s="23"/>
+      <c r="U47" s="23"/>
+      <c r="V47" s="23"/>
+      <c r="W47" s="23"/>
+      <c r="X47" s="23"/>
+      <c r="Y47" s="23"/>
+      <c r="Z47" s="24"/>
+    </row>
+    <row r="48" spans="1:26" ht="15.75" thickBot="1">
+      <c r="A48">
+        <v>17</v>
+      </c>
+      <c r="B48" t="s">
+        <v>32</v>
+      </c>
+      <c r="C48" t="s">
+        <v>19</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48">
+        <v>1</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>17</v>
+      </c>
+      <c r="K48" s="34"/>
+      <c r="L48" s="35"/>
+      <c r="M48" s="35"/>
+      <c r="N48" s="35"/>
+      <c r="O48" s="35"/>
+      <c r="P48" s="35"/>
+      <c r="Q48" s="35"/>
+      <c r="R48" s="41"/>
+      <c r="S48" s="34"/>
+      <c r="T48" s="35"/>
+      <c r="U48" s="35"/>
+      <c r="V48" s="35"/>
+      <c r="W48" s="35"/>
+      <c r="X48" s="35"/>
+      <c r="Y48" s="35"/>
+      <c r="Z48" s="36"/>
+    </row>
+    <row r="49" spans="5:26" ht="15.75" thickTop="1">
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="K49" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="L49" s="11"/>
+      <c r="M49" s="11"/>
+      <c r="N49" s="11"/>
+      <c r="O49" s="11"/>
+      <c r="P49" s="11"/>
+      <c r="Q49" s="11"/>
+      <c r="R49" s="11"/>
+      <c r="S49" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="T49" s="11"/>
+      <c r="U49" s="11"/>
+      <c r="V49" s="11"/>
+      <c r="W49" s="11"/>
+      <c r="X49" s="11"/>
+      <c r="Y49" s="11"/>
+      <c r="Z49" s="11"/>
+    </row>
+    <row r="50" spans="5:26">
+      <c r="E50" s="7"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+    </row>
+    <row r="51" spans="5:26">
+      <c r="E51" s="7"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
+    </row>
+    <row r="52" spans="5:26">
+      <c r="E52" s="7"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+    </row>
+    <row r="53" spans="5:26">
+      <c r="E53" s="7"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+    </row>
+    <row r="54" spans="5:26">
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+    </row>
+    <row r="55" spans="5:26">
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+    </row>
+    <row r="56" spans="5:26">
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+    </row>
+    <row r="57" spans="5:26">
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+    </row>
+    <row r="58" spans="5:26">
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+    </row>
+    <row r="59" spans="5:26">
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+    </row>
+    <row r="60" spans="5:26">
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+    </row>
+    <row r="61" spans="5:26">
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+    </row>
+    <row r="62" spans="5:26">
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+    </row>
+    <row r="63" spans="5:26">
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+    </row>
+    <row r="64" spans="5:26">
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+    </row>
+    <row r="65" spans="5:7">
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+    </row>
+    <row r="66" spans="5:7">
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+    </row>
+    <row r="67" spans="5:7">
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+    </row>
+    <row r="68" spans="5:7">
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
+    </row>
+    <row r="69" spans="5:7">
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
+    </row>
+    <row r="70" spans="5:7">
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+    </row>
+    <row r="71" spans="5:7">
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+    </row>
+    <row r="72" spans="5:7">
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3"/>
+    </row>
+    <row r="73" spans="5:7">
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
+    </row>
+    <row r="74" spans="5:7">
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+    </row>
+    <row r="75" spans="5:7">
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+    </row>
+    <row r="76" spans="5:7">
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3"/>
+    </row>
+    <row r="77" spans="5:7">
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="3"/>
+    </row>
+    <row r="78" spans="5:7">
+      <c r="E78" s="3"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="3"/>
+    </row>
+    <row r="79" spans="5:7">
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="3"/>
+    </row>
+    <row r="80" spans="5:7">
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
+      <c r="G80" s="3"/>
+    </row>
+    <row r="81" spans="5:7">
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="3"/>
+    </row>
+    <row r="82" spans="5:7">
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="3"/>
+    </row>
+    <row r="83" spans="5:7">
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3"/>
+    </row>
+    <row r="84" spans="5:7">
+      <c r="E84" s="3"/>
+      <c r="F84" s="3"/>
+      <c r="G84" s="3"/>
+    </row>
+    <row r="85" spans="5:7">
+      <c r="E85" s="3"/>
+      <c r="F85" s="3"/>
+      <c r="G85" s="3"/>
+    </row>
+    <row r="86" spans="5:7">
+      <c r="E86" s="3"/>
+      <c r="F86" s="3"/>
+      <c r="G86" s="3"/>
+    </row>
+    <row r="87" spans="5:7">
+      <c r="E87" s="3"/>
+      <c r="F87" s="3"/>
+      <c r="G87" s="3"/>
+    </row>
+    <row r="88" spans="5:7">
+      <c r="E88" s="3"/>
+      <c r="F88" s="3"/>
+      <c r="G88" s="3"/>
+    </row>
+    <row r="89" spans="5:7">
+      <c r="E89" s="3"/>
+      <c r="F89" s="3"/>
+      <c r="G89" s="3"/>
+    </row>
+    <row r="90" spans="5:7">
+      <c r="E90" s="3"/>
+      <c r="F90" s="3"/>
+      <c r="G90" s="3"/>
+    </row>
+    <row r="91" spans="5:7">
+      <c r="E91" s="3"/>
+      <c r="F91" s="3"/>
+      <c r="G91" s="3"/>
+    </row>
+    <row r="92" spans="5:7">
+      <c r="E92" s="3"/>
+      <c r="F92" s="3"/>
+      <c r="G92" s="3"/>
+    </row>
+    <row r="93" spans="5:7">
+      <c r="E93" s="3"/>
+      <c r="F93" s="3"/>
+      <c r="G93" s="3"/>
+    </row>
+    <row r="94" spans="5:7">
+      <c r="E94" s="3"/>
+      <c r="F94" s="3"/>
+      <c r="G94" s="3"/>
+    </row>
+    <row r="95" spans="5:7">
+      <c r="E95" s="3"/>
+      <c r="F95" s="3"/>
+      <c r="G95" s="3"/>
+    </row>
+    <row r="96" spans="5:7">
+      <c r="E96" s="3"/>
+      <c r="F96" s="3"/>
+      <c r="G96" s="3"/>
+    </row>
+    <row r="97" spans="5:7">
+      <c r="E97" s="3"/>
+      <c r="F97" s="3"/>
+      <c r="G97" s="3"/>
+    </row>
+    <row r="98" spans="5:7">
+      <c r="E98" s="3"/>
+      <c r="F98" s="3"/>
+      <c r="G98" s="3"/>
+    </row>
+    <row r="99" spans="5:7">
+      <c r="E99" s="3"/>
+      <c r="F99" s="3"/>
+      <c r="G99" s="3"/>
+    </row>
+    <row r="100" spans="5:7">
+      <c r="E100" s="3"/>
+      <c r="F100" s="3"/>
+      <c r="G100" s="3"/>
+    </row>
+    <row r="101" spans="5:7">
+      <c r="E101" s="3"/>
+      <c r="F101" s="3"/>
+      <c r="G101" s="3"/>
+    </row>
+    <row r="102" spans="5:7">
+      <c r="E102" s="3"/>
+      <c r="F102" s="3"/>
+      <c r="G102" s="3"/>
+    </row>
+    <row r="103" spans="5:7">
+      <c r="E103" s="3"/>
+      <c r="F103" s="3"/>
+      <c r="G103" s="3"/>
+    </row>
+    <row r="104" spans="5:7">
+      <c r="E104" s="3"/>
+      <c r="F104" s="3"/>
+      <c r="G104" s="3"/>
+    </row>
+    <row r="105" spans="5:7">
+      <c r="E105" s="3"/>
+      <c r="F105" s="3"/>
+      <c r="G105" s="3"/>
+    </row>
+    <row r="106" spans="5:7">
+      <c r="E106" s="3"/>
+      <c r="F106" s="3"/>
+      <c r="G106" s="3"/>
+    </row>
+    <row r="107" spans="5:7">
+      <c r="E107" s="3"/>
+      <c r="F107" s="3"/>
+      <c r="G107" s="3"/>
+    </row>
+    <row r="108" spans="5:7">
+      <c r="E108" s="3"/>
+      <c r="F108" s="3"/>
+      <c r="G108" s="3"/>
+    </row>
+    <row r="109" spans="5:7">
+      <c r="E109" s="3"/>
+      <c r="F109" s="3"/>
+      <c r="G109" s="3"/>
+    </row>
+    <row r="110" spans="5:7">
+      <c r="E110" s="3"/>
+      <c r="F110" s="3"/>
+      <c r="G110" s="3"/>
+    </row>
+    <row r="111" spans="5:7">
+      <c r="E111" s="3"/>
+      <c r="F111" s="3"/>
+      <c r="G111" s="3"/>
+    </row>
+    <row r="112" spans="5:7">
+      <c r="E112" s="3"/>
+      <c r="F112" s="3"/>
+      <c r="G112" s="3"/>
+    </row>
+    <row r="113" spans="5:7">
+      <c r="E113" s="3"/>
+      <c r="F113" s="3"/>
+      <c r="G113" s="3"/>
+    </row>
+    <row r="114" spans="5:7">
+      <c r="E114" s="3"/>
+      <c r="F114" s="3"/>
+      <c r="G114" s="3"/>
+    </row>
+    <row r="115" spans="5:7">
+      <c r="E115" s="3"/>
+      <c r="F115" s="3"/>
+      <c r="G115" s="3"/>
+    </row>
+    <row r="116" spans="5:7">
+      <c r="E116" s="3"/>
+      <c r="F116" s="3"/>
+      <c r="G116" s="3"/>
+    </row>
+    <row r="117" spans="5:7">
+      <c r="E117" s="3"/>
+      <c r="F117" s="3"/>
+      <c r="G117" s="3"/>
+    </row>
+    <row r="118" spans="5:7">
+      <c r="E118" s="3"/>
+      <c r="F118" s="3"/>
+      <c r="G118" s="3"/>
+    </row>
+    <row r="119" spans="5:7">
+      <c r="E119" s="3"/>
+      <c r="F119" s="3"/>
+      <c r="G119" s="3"/>
+    </row>
+    <row r="120" spans="5:7">
+      <c r="E120" s="3"/>
+      <c r="F120" s="3"/>
+      <c r="G120" s="3"/>
+    </row>
+    <row r="121" spans="5:7">
+      <c r="E121" s="3"/>
+      <c r="F121" s="3"/>
+      <c r="G121" s="3"/>
+    </row>
+    <row r="122" spans="5:7">
+      <c r="E122" s="3"/>
+      <c r="F122" s="3"/>
+      <c r="G122" s="3"/>
+    </row>
+    <row r="123" spans="5:7">
+      <c r="E123" s="3"/>
+      <c r="F123" s="3"/>
+      <c r="G123" s="3"/>
+    </row>
+    <row r="124" spans="5:7">
+      <c r="E124" s="3"/>
+      <c r="F124" s="3"/>
+      <c r="G124" s="3"/>
+    </row>
+    <row r="125" spans="5:7">
+      <c r="E125" s="3"/>
+      <c r="F125" s="3"/>
+      <c r="G125" s="3"/>
+    </row>
+    <row r="126" spans="5:7">
+      <c r="E126" s="3"/>
+      <c r="F126" s="3"/>
+      <c r="G126" s="3"/>
+    </row>
+    <row r="127" spans="5:7">
+      <c r="E127" s="3"/>
+      <c r="F127" s="3"/>
+      <c r="G127" s="3"/>
+    </row>
+    <row r="128" spans="5:7">
+      <c r="E128" s="3"/>
+      <c r="F128" s="3"/>
+      <c r="G128" s="3"/>
+    </row>
+    <row r="129" spans="5:7">
+      <c r="E129" s="3"/>
+      <c r="F129" s="3"/>
+      <c r="G129" s="3"/>
+    </row>
+    <row r="130" spans="5:7">
+      <c r="E130" s="3"/>
+      <c r="F130" s="3"/>
+      <c r="G130" s="3"/>
+    </row>
+    <row r="131" spans="5:7">
+      <c r="E131" s="3"/>
+      <c r="F131" s="3"/>
+      <c r="G131" s="3"/>
+    </row>
+    <row r="132" spans="5:7">
+      <c r="E132" s="3"/>
+      <c r="F132" s="3"/>
+      <c r="G132" s="3"/>
+    </row>
+    <row r="133" spans="5:7">
+      <c r="E133" s="3"/>
+      <c r="F133" s="3"/>
+      <c r="G133" s="3"/>
+    </row>
+    <row r="134" spans="5:7">
+      <c r="E134" s="3"/>
+      <c r="F134" s="3"/>
+      <c r="G134" s="3"/>
+    </row>
+    <row r="135" spans="5:7">
+      <c r="E135" s="3"/>
+      <c r="F135" s="3"/>
+      <c r="G135" s="3"/>
+    </row>
+    <row r="136" spans="5:7">
+      <c r="E136" s="3"/>
+      <c r="F136" s="3"/>
+      <c r="G136" s="3"/>
+    </row>
+    <row r="137" spans="5:7">
+      <c r="E137" s="3"/>
+      <c r="F137" s="3"/>
+      <c r="G137" s="3"/>
+    </row>
+    <row r="138" spans="5:7">
+      <c r="E138" s="3"/>
+      <c r="F138" s="3"/>
+      <c r="G138" s="3"/>
+    </row>
+    <row r="139" spans="5:7">
+      <c r="E139" s="3"/>
+      <c r="F139" s="3"/>
+      <c r="G139" s="3"/>
+    </row>
+    <row r="140" spans="5:7">
+      <c r="E140" s="3"/>
+      <c r="F140" s="3"/>
+      <c r="G140" s="3"/>
+    </row>
+    <row r="141" spans="5:7">
+      <c r="E141" s="3"/>
+      <c r="F141" s="3"/>
+      <c r="G141" s="3"/>
+    </row>
+    <row r="142" spans="5:7">
+      <c r="E142" s="3"/>
+      <c r="F142" s="3"/>
+      <c r="G142" s="3"/>
+    </row>
+    <row r="143" spans="5:7">
+      <c r="E143" s="3"/>
+      <c r="F143" s="3"/>
+      <c r="G143" s="3"/>
+    </row>
+    <row r="144" spans="5:7">
+      <c r="E144" s="3"/>
+      <c r="F144" s="3"/>
+      <c r="G144" s="3"/>
+    </row>
+    <row r="145" spans="5:7">
+      <c r="E145" s="3"/>
+      <c r="F145" s="3"/>
+      <c r="G145" s="3"/>
+    </row>
+    <row r="146" spans="5:7">
+      <c r="E146" s="3"/>
+      <c r="F146" s="3"/>
+      <c r="G146" s="3"/>
+    </row>
+    <row r="147" spans="5:7">
+      <c r="E147" s="3"/>
+      <c r="F147" s="3"/>
+      <c r="G147" s="3"/>
+    </row>
+    <row r="148" spans="5:7">
+      <c r="E148" s="3"/>
+      <c r="F148" s="3"/>
+      <c r="G148" s="3"/>
+    </row>
+    <row r="149" spans="5:7">
+      <c r="E149" s="3"/>
+      <c r="F149" s="3"/>
+      <c r="G149" s="3"/>
+    </row>
+    <row r="150" spans="5:7">
+      <c r="E150" s="3"/>
+      <c r="F150" s="3"/>
+      <c r="G150" s="3"/>
+    </row>
+    <row r="151" spans="5:7">
+      <c r="E151" s="3"/>
+      <c r="F151" s="3"/>
+      <c r="G151" s="3"/>
+    </row>
+    <row r="152" spans="5:7">
+      <c r="E152" s="3"/>
+      <c r="F152" s="3"/>
+      <c r="G152" s="3"/>
+    </row>
+    <row r="153" spans="5:7">
+      <c r="E153" s="3"/>
+      <c r="F153" s="3"/>
+      <c r="G153" s="3"/>
+    </row>
+    <row r="154" spans="5:7">
+      <c r="E154" s="3"/>
+      <c r="F154" s="3"/>
+      <c r="G154" s="3"/>
+    </row>
+    <row r="155" spans="5:7">
+      <c r="E155" s="3"/>
+      <c r="F155" s="3"/>
+      <c r="G155" s="3"/>
+    </row>
+    <row r="156" spans="5:7">
+      <c r="E156" s="3"/>
+      <c r="F156" s="3"/>
+      <c r="G156" s="3"/>
+    </row>
+    <row r="157" spans="5:7">
+      <c r="E157" s="3"/>
+      <c r="F157" s="3"/>
+      <c r="G157" s="3"/>
+    </row>
+    <row r="158" spans="5:7">
+      <c r="E158" s="3"/>
+      <c r="F158" s="3"/>
+      <c r="G158" s="3"/>
+    </row>
+    <row r="159" spans="5:7">
+      <c r="E159" s="3"/>
+      <c r="F159" s="3"/>
+      <c r="G159" s="3"/>
+    </row>
+    <row r="160" spans="5:7">
+      <c r="E160" s="3"/>
+      <c r="F160" s="3"/>
+      <c r="G160" s="3"/>
+    </row>
+    <row r="161" spans="5:7">
+      <c r="E161" s="3"/>
+      <c r="F161" s="3"/>
+      <c r="G161" s="3"/>
+    </row>
+    <row r="162" spans="5:7">
+      <c r="E162" s="3"/>
+      <c r="F162" s="3"/>
+      <c r="G162" s="3"/>
+    </row>
+    <row r="163" spans="5:7">
+      <c r="E163" s="3"/>
+      <c r="F163" s="3"/>
+      <c r="G163" s="3"/>
+    </row>
+    <row r="164" spans="5:7">
+      <c r="E164" s="3"/>
+      <c r="F164" s="3"/>
+      <c r="G164" s="3"/>
+    </row>
+    <row r="165" spans="5:7">
+      <c r="E165" s="3"/>
+      <c r="F165" s="3"/>
+      <c r="G165" s="3"/>
+    </row>
+    <row r="166" spans="5:7">
+      <c r="E166" s="3"/>
+      <c r="F166" s="3"/>
+      <c r="G166" s="3"/>
+    </row>
+    <row r="167" spans="5:7">
+      <c r="E167" s="3"/>
+      <c r="F167" s="3"/>
+      <c r="G167" s="3"/>
+    </row>
+    <row r="168" spans="5:7">
+      <c r="E168" s="3"/>
+      <c r="F168" s="3"/>
+      <c r="G168" s="3"/>
+    </row>
+    <row r="169" spans="5:7">
+      <c r="E169" s="3"/>
+      <c r="F169" s="3"/>
+      <c r="G169" s="3"/>
+    </row>
+    <row r="170" spans="5:7">
+      <c r="E170" s="3"/>
+      <c r="F170" s="3"/>
+      <c r="G170" s="3"/>
+    </row>
+    <row r="171" spans="5:7">
+      <c r="E171" s="3"/>
+      <c r="F171" s="3"/>
+      <c r="G171" s="3"/>
+    </row>
+    <row r="172" spans="5:7">
+      <c r="E172" s="3"/>
+      <c r="F172" s="3"/>
+      <c r="G172" s="3"/>
+    </row>
+    <row r="173" spans="5:7">
+      <c r="E173" s="3"/>
+      <c r="F173" s="3"/>
+      <c r="G173" s="3"/>
+    </row>
+    <row r="174" spans="5:7">
+      <c r="E174" s="3"/>
+      <c r="F174" s="3"/>
+      <c r="G174" s="3"/>
+    </row>
+    <row r="175" spans="5:7">
+      <c r="E175" s="3"/>
+      <c r="F175" s="3"/>
+      <c r="G175" s="3"/>
+    </row>
+    <row r="176" spans="5:7">
+      <c r="E176" s="3"/>
+      <c r="F176" s="3"/>
+      <c r="G176" s="3"/>
+    </row>
+    <row r="177" spans="5:7">
+      <c r="E177" s="3"/>
+      <c r="F177" s="3"/>
+      <c r="G177" s="3"/>
+    </row>
+    <row r="178" spans="5:7">
+      <c r="E178" s="3"/>
+      <c r="F178" s="3"/>
+      <c r="G178" s="3"/>
+    </row>
+    <row r="179" spans="5:7">
+      <c r="E179" s="3"/>
+      <c r="F179" s="3"/>
+      <c r="G179" s="3"/>
+    </row>
+    <row r="180" spans="5:7">
+      <c r="E180" s="3"/>
+      <c r="F180" s="3"/>
+      <c r="G180" s="3"/>
+    </row>
+    <row r="181" spans="5:7">
+      <c r="E181" s="3"/>
+      <c r="F181" s="3"/>
+      <c r="G181" s="3"/>
+    </row>
+    <row r="182" spans="5:7">
+      <c r="E182" s="3"/>
+      <c r="F182" s="3"/>
+      <c r="G182" s="3"/>
+    </row>
+    <row r="183" spans="5:7">
+      <c r="E183" s="3"/>
+      <c r="F183" s="3"/>
+      <c r="G183" s="3"/>
+    </row>
+    <row r="184" spans="5:7">
+      <c r="E184" s="3"/>
+      <c r="F184" s="3"/>
+      <c r="G184" s="3"/>
+    </row>
+    <row r="185" spans="5:7">
+      <c r="E185" s="3"/>
+      <c r="F185" s="3"/>
+      <c r="G185" s="3"/>
+    </row>
+    <row r="186" spans="5:7">
+      <c r="E186" s="3"/>
+      <c r="F186" s="3"/>
+      <c r="G186" s="3"/>
+    </row>
+    <row r="187" spans="5:7">
+      <c r="E187" s="3"/>
+      <c r="F187" s="3"/>
+      <c r="G187" s="3"/>
+    </row>
+    <row r="188" spans="5:7">
+      <c r="E188" s="3"/>
+      <c r="F188" s="3"/>
+      <c r="G188" s="3"/>
+    </row>
+    <row r="189" spans="5:7">
+      <c r="E189" s="3"/>
+      <c r="F189" s="3"/>
+      <c r="G189" s="3"/>
+    </row>
+    <row r="190" spans="5:7">
+      <c r="E190" s="3"/>
+      <c r="F190" s="3"/>
+      <c r="G190" s="3"/>
+    </row>
+    <row r="191" spans="5:7">
+      <c r="E191" s="3"/>
+      <c r="F191" s="3"/>
+      <c r="G191" s="3"/>
+    </row>
+    <row r="192" spans="5:7">
+      <c r="E192" s="3"/>
+      <c r="F192" s="3"/>
+      <c r="G192" s="3"/>
+    </row>
+    <row r="193" spans="5:7">
+      <c r="E193" s="3"/>
+      <c r="F193" s="3"/>
+      <c r="G193" s="3"/>
+    </row>
+    <row r="194" spans="5:7">
+      <c r="E194" s="3"/>
+      <c r="F194" s="3"/>
+      <c r="G194" s="3"/>
+    </row>
+    <row r="195" spans="5:7">
+      <c r="E195" s="3"/>
+      <c r="F195" s="3"/>
+      <c r="G195" s="3"/>
+    </row>
+    <row r="196" spans="5:7">
+      <c r="E196" s="3"/>
+      <c r="F196" s="3"/>
+      <c r="G196" s="3"/>
+    </row>
+    <row r="197" spans="5:7">
+      <c r="E197" s="3"/>
+      <c r="F197" s="3"/>
+      <c r="G197" s="3"/>
+    </row>
+    <row r="198" spans="5:7">
+      <c r="E198" s="3"/>
+      <c r="F198" s="3"/>
+      <c r="G198" s="3"/>
+    </row>
+    <row r="199" spans="5:7">
+      <c r="E199" s="3"/>
+      <c r="F199" s="3"/>
+      <c r="G199" s="3"/>
+    </row>
+    <row r="200" spans="5:7">
+      <c r="E200" s="3"/>
+      <c r="F200" s="3"/>
+      <c r="G200" s="3"/>
+    </row>
+    <row r="201" spans="5:7">
+      <c r="E201" s="3"/>
+      <c r="F201" s="3"/>
+      <c r="G201" s="3"/>
+    </row>
+    <row r="202" spans="5:7">
+      <c r="E202" s="3"/>
+      <c r="F202" s="3"/>
+      <c r="G202" s="3"/>
+    </row>
+    <row r="203" spans="5:7">
+      <c r="E203" s="3"/>
+      <c r="F203" s="3"/>
+      <c r="G203" s="3"/>
+    </row>
+    <row r="204" spans="5:7">
+      <c r="E204" s="3"/>
+      <c r="F204" s="3"/>
+      <c r="G204" s="3"/>
+    </row>
+    <row r="205" spans="5:7">
+      <c r="E205" s="3"/>
+      <c r="F205" s="3"/>
+      <c r="G205" s="3"/>
+    </row>
+    <row r="206" spans="5:7">
+      <c r="E206" s="3"/>
+      <c r="F206" s="3"/>
+      <c r="G206" s="3"/>
+    </row>
+    <row r="207" spans="5:7">
+      <c r="E207" s="3"/>
+      <c r="F207" s="3"/>
+      <c r="G207" s="3"/>
+    </row>
+    <row r="208" spans="5:7">
+      <c r="E208" s="3"/>
+      <c r="F208" s="3"/>
+      <c r="G208" s="3"/>
+    </row>
+    <row r="209" spans="5:7">
+      <c r="E209" s="3"/>
+      <c r="F209" s="3"/>
+      <c r="G209" s="3"/>
+    </row>
+    <row r="210" spans="5:7">
+      <c r="E210" s="3"/>
+      <c r="F210" s="3"/>
+      <c r="G210" s="3"/>
+    </row>
+    <row r="211" spans="5:7">
+      <c r="E211" s="3"/>
+      <c r="F211" s="3"/>
+      <c r="G211" s="3"/>
+    </row>
+    <row r="212" spans="5:7">
+      <c r="E212" s="3"/>
+      <c r="F212" s="3"/>
+      <c r="G212" s="3"/>
+    </row>
+    <row r="213" spans="5:7">
+      <c r="E213" s="3"/>
+      <c r="F213" s="3"/>
+      <c r="G213" s="3"/>
+    </row>
+    <row r="214" spans="5:7">
+      <c r="E214" s="3"/>
+      <c r="F214" s="3"/>
+      <c r="G214" s="3"/>
+    </row>
+    <row r="215" spans="5:7">
+      <c r="E215" s="3"/>
+      <c r="F215" s="3"/>
+      <c r="G215" s="3"/>
+    </row>
+    <row r="216" spans="5:7">
+      <c r="E216" s="3"/>
+      <c r="F216" s="3"/>
+      <c r="G216" s="3"/>
+    </row>
+    <row r="217" spans="5:7">
+      <c r="E217" s="3"/>
+      <c r="F217" s="3"/>
+      <c r="G217" s="3"/>
+    </row>
+    <row r="218" spans="5:7">
+      <c r="E218" s="3"/>
+      <c r="F218" s="3"/>
+      <c r="G218" s="3"/>
+    </row>
+    <row r="219" spans="5:7">
+      <c r="E219" s="3"/>
+      <c r="F219" s="3"/>
+      <c r="G219" s="3"/>
+    </row>
+    <row r="220" spans="5:7">
+      <c r="E220" s="3"/>
+      <c r="F220" s="3"/>
+      <c r="G220" s="3"/>
+    </row>
+    <row r="221" spans="5:7">
+      <c r="E221" s="3"/>
+      <c r="F221" s="3"/>
+      <c r="G221" s="3"/>
+    </row>
+    <row r="222" spans="5:7">
+      <c r="E222" s="3"/>
+      <c r="F222" s="3"/>
+      <c r="G222" s="3"/>
+    </row>
+    <row r="223" spans="5:7">
+      <c r="E223" s="3"/>
+      <c r="F223" s="3"/>
+      <c r="G223" s="3"/>
+    </row>
+    <row r="224" spans="5:7">
+      <c r="E224" s="3"/>
+      <c r="F224" s="3"/>
+      <c r="G224" s="3"/>
+    </row>
+    <row r="225" spans="5:7">
+      <c r="E225" s="3"/>
+      <c r="F225" s="3"/>
+      <c r="G225" s="3"/>
+    </row>
+    <row r="226" spans="5:7">
+      <c r="E226" s="3"/>
+      <c r="F226" s="3"/>
+      <c r="G226" s="3"/>
+    </row>
+    <row r="227" spans="5:7">
+      <c r="E227" s="3"/>
+      <c r="F227" s="3"/>
+      <c r="G227" s="3"/>
+    </row>
+    <row r="228" spans="5:7">
+      <c r="E228" s="3"/>
+      <c r="F228" s="3"/>
+      <c r="G228" s="3"/>
+    </row>
+    <row r="229" spans="5:7">
+      <c r="E229" s="3"/>
+      <c r="F229" s="3"/>
+      <c r="G229" s="3"/>
+    </row>
+    <row r="230" spans="5:7">
+      <c r="E230" s="3"/>
+      <c r="F230" s="3"/>
+      <c r="G230" s="3"/>
+    </row>
+    <row r="231" spans="5:7">
+      <c r="E231" s="3"/>
+      <c r="F231" s="3"/>
+      <c r="G231" s="3"/>
+    </row>
+    <row r="232" spans="5:7">
+      <c r="E232" s="3"/>
+      <c r="F232" s="3"/>
+      <c r="G232" s="3"/>
+    </row>
+    <row r="233" spans="5:7">
+      <c r="E233" s="3"/>
+      <c r="F233" s="3"/>
+      <c r="G233" s="3"/>
+    </row>
+    <row r="234" spans="5:7">
+      <c r="E234" s="3"/>
+      <c r="F234" s="3"/>
+      <c r="G234" s="3"/>
+    </row>
+    <row r="235" spans="5:7">
+      <c r="E235" s="3"/>
+      <c r="F235" s="3"/>
+      <c r="G235" s="3"/>
+    </row>
+    <row r="236" spans="5:7">
+      <c r="E236" s="3"/>
+      <c r="F236" s="3"/>
+      <c r="G236" s="3"/>
+    </row>
+    <row r="237" spans="5:7">
+      <c r="E237" s="3"/>
+      <c r="F237" s="3"/>
+      <c r="G237" s="3"/>
+    </row>
+    <row r="238" spans="5:7">
+      <c r="E238" s="3"/>
+      <c r="F238" s="3"/>
+      <c r="G238" s="3"/>
+    </row>
+    <row r="239" spans="5:7">
+      <c r="E239" s="3"/>
+      <c r="F239" s="3"/>
+      <c r="G239" s="3"/>
+    </row>
+    <row r="240" spans="5:7">
+      <c r="E240" s="3"/>
+      <c r="F240" s="3"/>
+      <c r="G240" s="3"/>
+    </row>
+    <row r="241" spans="5:7">
+      <c r="E241" s="3"/>
+      <c r="F241" s="3"/>
+      <c r="G241" s="3"/>
+    </row>
+    <row r="242" spans="5:7">
+      <c r="E242" s="3"/>
+      <c r="F242" s="3"/>
+      <c r="G242" s="3"/>
+    </row>
+    <row r="243" spans="5:7">
+      <c r="E243" s="3"/>
+      <c r="F243" s="3"/>
+      <c r="G243" s="3"/>
+    </row>
+    <row r="244" spans="5:7">
+      <c r="E244" s="3"/>
+      <c r="F244" s="3"/>
+      <c r="G244" s="3"/>
+    </row>
+    <row r="245" spans="5:7">
+      <c r="E245" s="3"/>
+      <c r="F245" s="3"/>
+      <c r="G245" s="3"/>
+    </row>
+    <row r="246" spans="5:7">
+      <c r="E246" s="3"/>
+      <c r="F246" s="3"/>
+      <c r="G246" s="3"/>
+    </row>
+    <row r="247" spans="5:7">
+      <c r="E247" s="3"/>
+      <c r="F247" s="3"/>
+      <c r="G247" s="3"/>
+    </row>
+    <row r="248" spans="5:7">
+      <c r="E248" s="3"/>
+      <c r="F248" s="3"/>
+      <c r="G248" s="3"/>
+    </row>
+    <row r="249" spans="5:7">
+      <c r="E249" s="3"/>
+      <c r="F249" s="3"/>
+      <c r="G249" s="3"/>
+    </row>
+    <row r="250" spans="5:7">
+      <c r="E250" s="3"/>
+      <c r="F250" s="3"/>
+      <c r="G250" s="3"/>
+    </row>
+    <row r="251" spans="5:7">
+      <c r="E251" s="3"/>
+      <c r="F251" s="3"/>
+      <c r="G251" s="3"/>
+    </row>
+    <row r="252" spans="5:7">
+      <c r="E252" s="3"/>
+      <c r="F252" s="3"/>
+      <c r="G252" s="3"/>
+    </row>
+    <row r="253" spans="5:7">
+      <c r="E253" s="3"/>
+      <c r="F253" s="3"/>
+      <c r="G253" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="19">
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="K32:R32"/>
+    <mergeCell ref="S32:Z32"/>
+    <mergeCell ref="K33:L34"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="O33:O34"/>
+    <mergeCell ref="P33:P34"/>
+    <mergeCell ref="K35:L36"/>
+    <mergeCell ref="K37:L39"/>
+    <mergeCell ref="M37:M39"/>
+    <mergeCell ref="M35:M36"/>
+    <mergeCell ref="N35:O36"/>
+    <mergeCell ref="K49:R49"/>
+    <mergeCell ref="S49:Z49"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A31:C31"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="F52:G52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Some models + Floor_1 textures
</commit_message>
<xml_diff>
--- a/Design/Assets.xlsx
+++ b/Design/Assets.xlsx
@@ -613,55 +613,16 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -671,30 +632,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -720,6 +657,69 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1017,9 +1017,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P38" sqref="P38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1060,11 +1060,11 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3">
@@ -1313,7 +1313,7 @@
         <v>4</v>
       </c>
       <c r="F13" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G13" s="3">
         <v>0.5</v>
@@ -1336,7 +1336,7 @@
         <v>4</v>
       </c>
       <c r="F14" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G14" s="3">
         <v>1</v>
@@ -1603,11 +1603,11 @@
       <c r="G30" s="3"/>
     </row>
     <row r="31" spans="1:26" s="1" customFormat="1">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
@@ -1644,26 +1644,26 @@
       <c r="J32">
         <v>1</v>
       </c>
-      <c r="K32" s="10" t="s">
+      <c r="K32" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="L32" s="10"/>
-      <c r="M32" s="10"/>
-      <c r="N32" s="10"/>
-      <c r="O32" s="10"/>
-      <c r="P32" s="10"/>
-      <c r="Q32" s="10"/>
-      <c r="R32" s="10"/>
-      <c r="S32" s="10" t="s">
+      <c r="L32" s="22"/>
+      <c r="M32" s="22"/>
+      <c r="N32" s="22"/>
+      <c r="O32" s="22"/>
+      <c r="P32" s="22"/>
+      <c r="Q32" s="22"/>
+      <c r="R32" s="22"/>
+      <c r="S32" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="T32" s="10"/>
-      <c r="U32" s="10"/>
-      <c r="V32" s="10"/>
-      <c r="W32" s="10"/>
-      <c r="X32" s="10"/>
-      <c r="Y32" s="10"/>
-      <c r="Z32" s="10"/>
+      <c r="T32" s="22"/>
+      <c r="U32" s="22"/>
+      <c r="V32" s="22"/>
+      <c r="W32" s="22"/>
+      <c r="X32" s="22"/>
+      <c r="Y32" s="22"/>
+      <c r="Z32" s="22"/>
     </row>
     <row r="33" spans="1:26" ht="15.75" thickTop="1">
       <c r="A33">
@@ -1694,36 +1694,36 @@
       <c r="J33">
         <v>2</v>
       </c>
-      <c r="K33" s="12">
-        <v>1</v>
-      </c>
-      <c r="L33" s="13"/>
-      <c r="M33" s="14">
+      <c r="K33" s="23">
+        <v>1</v>
+      </c>
+      <c r="L33" s="24"/>
+      <c r="M33" s="7">
         <v>2</v>
       </c>
-      <c r="N33" s="14">
+      <c r="N33" s="7">
         <v>6</v>
       </c>
-      <c r="O33" s="15">
+      <c r="O33" s="29">
         <v>4</v>
       </c>
-      <c r="P33" s="15">
+      <c r="P33" s="29">
         <v>5</v>
       </c>
-      <c r="Q33" s="14">
+      <c r="Q33" s="7">
         <v>7</v>
       </c>
-      <c r="R33" s="16">
+      <c r="R33" s="8">
         <v>15</v>
       </c>
-      <c r="S33" s="17"/>
-      <c r="T33" s="14"/>
-      <c r="U33" s="14"/>
-      <c r="V33" s="14"/>
-      <c r="W33" s="14"/>
-      <c r="X33" s="14"/>
-      <c r="Y33" s="14"/>
-      <c r="Z33" s="16"/>
+      <c r="S33" s="9"/>
+      <c r="T33" s="7"/>
+      <c r="U33" s="7"/>
+      <c r="V33" s="7"/>
+      <c r="W33" s="7"/>
+      <c r="X33" s="7"/>
+      <c r="Y33" s="7"/>
+      <c r="Z33" s="8"/>
     </row>
     <row r="34" spans="1:26">
       <c r="A34">
@@ -1754,24 +1754,24 @@
       <c r="J34">
         <v>3</v>
       </c>
-      <c r="K34" s="18"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="20">
+      <c r="K34" s="25"/>
+      <c r="L34" s="26"/>
+      <c r="M34" s="27">
         <v>3</v>
       </c>
-      <c r="N34" s="21"/>
-      <c r="O34" s="22"/>
-      <c r="P34" s="22"/>
-      <c r="Q34" s="23"/>
-      <c r="R34" s="24"/>
-      <c r="S34" s="25"/>
-      <c r="T34" s="23"/>
-      <c r="U34" s="23"/>
-      <c r="V34" s="23"/>
-      <c r="W34" s="23"/>
-      <c r="X34" s="23"/>
-      <c r="Y34" s="23"/>
-      <c r="Z34" s="24"/>
+      <c r="N34" s="28"/>
+      <c r="O34" s="30"/>
+      <c r="P34" s="30"/>
+      <c r="Q34" s="10"/>
+      <c r="R34" s="11"/>
+      <c r="S34" s="12"/>
+      <c r="T34" s="10"/>
+      <c r="U34" s="10"/>
+      <c r="V34" s="10"/>
+      <c r="W34" s="10"/>
+      <c r="X34" s="10"/>
+      <c r="Y34" s="10"/>
+      <c r="Z34" s="11"/>
     </row>
     <row r="35" spans="1:26">
       <c r="A35">
@@ -1802,28 +1802,28 @@
       <c r="J35">
         <v>4</v>
       </c>
-      <c r="K35" s="26">
+      <c r="K35" s="31">
         <v>8</v>
       </c>
-      <c r="L35" s="27"/>
-      <c r="M35" s="28">
+      <c r="L35" s="32"/>
+      <c r="M35" s="35">
         <v>13</v>
       </c>
-      <c r="N35" s="29">
+      <c r="N35" s="37">
         <v>14</v>
       </c>
-      <c r="O35" s="27"/>
-      <c r="P35" s="23"/>
-      <c r="Q35" s="23"/>
-      <c r="R35" s="24"/>
-      <c r="S35" s="25"/>
-      <c r="T35" s="23"/>
-      <c r="U35" s="23"/>
-      <c r="V35" s="23"/>
-      <c r="W35" s="23"/>
-      <c r="X35" s="23"/>
-      <c r="Y35" s="23"/>
-      <c r="Z35" s="24"/>
+      <c r="O35" s="32"/>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="10"/>
+      <c r="R35" s="11"/>
+      <c r="S35" s="12"/>
+      <c r="T35" s="10"/>
+      <c r="U35" s="10"/>
+      <c r="V35" s="10"/>
+      <c r="W35" s="10"/>
+      <c r="X35" s="10"/>
+      <c r="Y35" s="10"/>
+      <c r="Z35" s="11"/>
     </row>
     <row r="36" spans="1:26">
       <c r="A36">
@@ -1854,22 +1854,22 @@
       <c r="J36">
         <v>5</v>
       </c>
-      <c r="K36" s="18"/>
-      <c r="L36" s="19"/>
-      <c r="M36" s="22"/>
-      <c r="N36" s="30"/>
-      <c r="O36" s="19"/>
-      <c r="P36" s="23"/>
-      <c r="Q36" s="23"/>
-      <c r="R36" s="24"/>
-      <c r="S36" s="25"/>
-      <c r="T36" s="23"/>
-      <c r="U36" s="23"/>
-      <c r="V36" s="23"/>
-      <c r="W36" s="23"/>
-      <c r="X36" s="23"/>
-      <c r="Y36" s="23"/>
-      <c r="Z36" s="24"/>
+      <c r="K36" s="25"/>
+      <c r="L36" s="26"/>
+      <c r="M36" s="30"/>
+      <c r="N36" s="38"/>
+      <c r="O36" s="26"/>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="10"/>
+      <c r="R36" s="11"/>
+      <c r="S36" s="12"/>
+      <c r="T36" s="10"/>
+      <c r="U36" s="10"/>
+      <c r="V36" s="10"/>
+      <c r="W36" s="10"/>
+      <c r="X36" s="10"/>
+      <c r="Y36" s="10"/>
+      <c r="Z36" s="11"/>
     </row>
     <row r="37" spans="1:26">
       <c r="A37">
@@ -1900,26 +1900,26 @@
       <c r="J37">
         <v>6</v>
       </c>
-      <c r="K37" s="26">
+      <c r="K37" s="31">
         <v>9</v>
       </c>
-      <c r="L37" s="27"/>
-      <c r="M37" s="28">
+      <c r="L37" s="32"/>
+      <c r="M37" s="35">
         <v>10</v>
       </c>
-      <c r="N37" s="23"/>
-      <c r="O37" s="23"/>
-      <c r="P37" s="23"/>
-      <c r="Q37" s="23"/>
-      <c r="R37" s="24"/>
-      <c r="S37" s="25"/>
-      <c r="T37" s="23"/>
-      <c r="U37" s="23"/>
-      <c r="V37" s="23"/>
-      <c r="W37" s="23"/>
-      <c r="X37" s="23"/>
-      <c r="Y37" s="23"/>
-      <c r="Z37" s="24"/>
+      <c r="N37" s="10"/>
+      <c r="O37" s="10"/>
+      <c r="P37" s="10"/>
+      <c r="Q37" s="10"/>
+      <c r="R37" s="11"/>
+      <c r="S37" s="12"/>
+      <c r="T37" s="10"/>
+      <c r="U37" s="10"/>
+      <c r="V37" s="10"/>
+      <c r="W37" s="10"/>
+      <c r="X37" s="10"/>
+      <c r="Y37" s="10"/>
+      <c r="Z37" s="11"/>
     </row>
     <row r="38" spans="1:26">
       <c r="A38">
@@ -1950,22 +1950,22 @@
       <c r="J38">
         <v>7</v>
       </c>
-      <c r="K38" s="31"/>
-      <c r="L38" s="32"/>
-      <c r="M38" s="33"/>
-      <c r="N38" s="23"/>
-      <c r="O38" s="23"/>
-      <c r="P38" s="23"/>
-      <c r="Q38" s="23"/>
-      <c r="R38" s="24"/>
-      <c r="S38" s="25"/>
-      <c r="T38" s="23"/>
-      <c r="U38" s="23"/>
-      <c r="V38" s="23"/>
-      <c r="W38" s="23"/>
-      <c r="X38" s="23"/>
-      <c r="Y38" s="23"/>
-      <c r="Z38" s="24"/>
+      <c r="K38" s="33"/>
+      <c r="L38" s="34"/>
+      <c r="M38" s="36"/>
+      <c r="N38" s="10"/>
+      <c r="O38" s="10"/>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="10"/>
+      <c r="R38" s="11"/>
+      <c r="S38" s="12"/>
+      <c r="T38" s="10"/>
+      <c r="U38" s="10"/>
+      <c r="V38" s="10"/>
+      <c r="W38" s="10"/>
+      <c r="X38" s="10"/>
+      <c r="Y38" s="10"/>
+      <c r="Z38" s="11"/>
     </row>
     <row r="39" spans="1:26">
       <c r="A39">
@@ -1996,22 +1996,22 @@
       <c r="J39">
         <v>8</v>
       </c>
-      <c r="K39" s="18"/>
-      <c r="L39" s="19"/>
-      <c r="M39" s="22"/>
-      <c r="N39" s="23"/>
-      <c r="O39" s="23"/>
-      <c r="P39" s="23"/>
-      <c r="Q39" s="23"/>
-      <c r="R39" s="24"/>
-      <c r="S39" s="25"/>
-      <c r="T39" s="23"/>
-      <c r="U39" s="23"/>
-      <c r="V39" s="23"/>
-      <c r="W39" s="23"/>
-      <c r="X39" s="23"/>
-      <c r="Y39" s="23"/>
-      <c r="Z39" s="24"/>
+      <c r="K39" s="25"/>
+      <c r="L39" s="26"/>
+      <c r="M39" s="30"/>
+      <c r="N39" s="10"/>
+      <c r="O39" s="10"/>
+      <c r="P39" s="10"/>
+      <c r="Q39" s="10"/>
+      <c r="R39" s="11"/>
+      <c r="S39" s="12"/>
+      <c r="T39" s="10"/>
+      <c r="U39" s="10"/>
+      <c r="V39" s="10"/>
+      <c r="W39" s="10"/>
+      <c r="X39" s="10"/>
+      <c r="Y39" s="10"/>
+      <c r="Z39" s="11"/>
     </row>
     <row r="40" spans="1:26" ht="15.75" thickBot="1">
       <c r="A40">
@@ -2042,26 +2042,26 @@
       <c r="J40">
         <v>9</v>
       </c>
-      <c r="K40" s="34">
+      <c r="K40" s="13">
         <v>11</v>
       </c>
-      <c r="L40" s="35">
+      <c r="L40" s="14">
         <v>12</v>
       </c>
-      <c r="M40" s="35"/>
-      <c r="N40" s="35"/>
-      <c r="O40" s="35"/>
-      <c r="P40" s="35"/>
-      <c r="Q40" s="35"/>
-      <c r="R40" s="36"/>
-      <c r="S40" s="34"/>
-      <c r="T40" s="35"/>
-      <c r="U40" s="35"/>
-      <c r="V40" s="35"/>
-      <c r="W40" s="35"/>
-      <c r="X40" s="35"/>
-      <c r="Y40" s="35"/>
-      <c r="Z40" s="36"/>
+      <c r="M40" s="14"/>
+      <c r="N40" s="14"/>
+      <c r="O40" s="14"/>
+      <c r="P40" s="14"/>
+      <c r="Q40" s="14"/>
+      <c r="R40" s="15"/>
+      <c r="S40" s="13"/>
+      <c r="T40" s="14"/>
+      <c r="U40" s="14"/>
+      <c r="V40" s="14"/>
+      <c r="W40" s="14"/>
+      <c r="X40" s="14"/>
+      <c r="Y40" s="14"/>
+      <c r="Z40" s="15"/>
     </row>
     <row r="41" spans="1:26" ht="15.75" thickTop="1">
       <c r="A41">
@@ -2092,22 +2092,22 @@
       <c r="J41">
         <v>10</v>
       </c>
-      <c r="K41" s="37"/>
-      <c r="L41" s="38"/>
-      <c r="M41" s="38"/>
-      <c r="N41" s="38"/>
-      <c r="O41" s="38"/>
-      <c r="P41" s="38"/>
-      <c r="Q41" s="38"/>
-      <c r="R41" s="39"/>
-      <c r="S41" s="17"/>
-      <c r="T41" s="14"/>
-      <c r="U41" s="14"/>
-      <c r="V41" s="14"/>
-      <c r="W41" s="14"/>
-      <c r="X41" s="14"/>
-      <c r="Y41" s="14"/>
-      <c r="Z41" s="16"/>
+      <c r="K41" s="16"/>
+      <c r="L41" s="17"/>
+      <c r="M41" s="17"/>
+      <c r="N41" s="17"/>
+      <c r="O41" s="17"/>
+      <c r="P41" s="17"/>
+      <c r="Q41" s="17"/>
+      <c r="R41" s="18"/>
+      <c r="S41" s="9"/>
+      <c r="T41" s="7"/>
+      <c r="U41" s="7"/>
+      <c r="V41" s="7"/>
+      <c r="W41" s="7"/>
+      <c r="X41" s="7"/>
+      <c r="Y41" s="7"/>
+      <c r="Z41" s="8"/>
     </row>
     <row r="42" spans="1:26">
       <c r="A42">
@@ -2138,22 +2138,22 @@
       <c r="J42">
         <v>11</v>
       </c>
-      <c r="K42" s="25"/>
-      <c r="L42" s="23"/>
-      <c r="M42" s="23"/>
-      <c r="N42" s="23"/>
-      <c r="O42" s="23"/>
-      <c r="P42" s="23"/>
-      <c r="Q42" s="23"/>
-      <c r="R42" s="40"/>
-      <c r="S42" s="25"/>
-      <c r="T42" s="23"/>
-      <c r="U42" s="23"/>
-      <c r="V42" s="23"/>
-      <c r="W42" s="23"/>
-      <c r="X42" s="23"/>
-      <c r="Y42" s="23"/>
-      <c r="Z42" s="24"/>
+      <c r="K42" s="12"/>
+      <c r="L42" s="10"/>
+      <c r="M42" s="10"/>
+      <c r="N42" s="10"/>
+      <c r="O42" s="10"/>
+      <c r="P42" s="10"/>
+      <c r="Q42" s="10"/>
+      <c r="R42" s="19"/>
+      <c r="S42" s="12"/>
+      <c r="T42" s="10"/>
+      <c r="U42" s="10"/>
+      <c r="V42" s="10"/>
+      <c r="W42" s="10"/>
+      <c r="X42" s="10"/>
+      <c r="Y42" s="10"/>
+      <c r="Z42" s="11"/>
     </row>
     <row r="43" spans="1:26">
       <c r="A43">
@@ -2184,22 +2184,22 @@
       <c r="J43">
         <v>12</v>
       </c>
-      <c r="K43" s="25"/>
-      <c r="L43" s="23"/>
-      <c r="M43" s="23"/>
-      <c r="N43" s="23"/>
-      <c r="O43" s="23"/>
-      <c r="P43" s="23"/>
-      <c r="Q43" s="23"/>
-      <c r="R43" s="40"/>
-      <c r="S43" s="25"/>
-      <c r="T43" s="23"/>
-      <c r="U43" s="23"/>
-      <c r="V43" s="23"/>
-      <c r="W43" s="23"/>
-      <c r="X43" s="23"/>
-      <c r="Y43" s="23"/>
-      <c r="Z43" s="24"/>
+      <c r="K43" s="12"/>
+      <c r="L43" s="10"/>
+      <c r="M43" s="10"/>
+      <c r="N43" s="10"/>
+      <c r="O43" s="10"/>
+      <c r="P43" s="10"/>
+      <c r="Q43" s="10"/>
+      <c r="R43" s="19"/>
+      <c r="S43" s="12"/>
+      <c r="T43" s="10"/>
+      <c r="U43" s="10"/>
+      <c r="V43" s="10"/>
+      <c r="W43" s="10"/>
+      <c r="X43" s="10"/>
+      <c r="Y43" s="10"/>
+      <c r="Z43" s="11"/>
     </row>
     <row r="44" spans="1:26">
       <c r="A44">
@@ -2230,22 +2230,22 @@
       <c r="J44">
         <v>13</v>
       </c>
-      <c r="K44" s="25"/>
-      <c r="L44" s="23"/>
-      <c r="M44" s="23"/>
-      <c r="N44" s="23"/>
-      <c r="O44" s="23"/>
-      <c r="P44" s="23"/>
-      <c r="Q44" s="23"/>
-      <c r="R44" s="40"/>
-      <c r="S44" s="25"/>
-      <c r="T44" s="23"/>
-      <c r="U44" s="23"/>
-      <c r="V44" s="23"/>
-      <c r="W44" s="23"/>
-      <c r="X44" s="23"/>
-      <c r="Y44" s="23"/>
-      <c r="Z44" s="24"/>
+      <c r="K44" s="12"/>
+      <c r="L44" s="10"/>
+      <c r="M44" s="10"/>
+      <c r="N44" s="10"/>
+      <c r="O44" s="10"/>
+      <c r="P44" s="10"/>
+      <c r="Q44" s="10"/>
+      <c r="R44" s="19"/>
+      <c r="S44" s="12"/>
+      <c r="T44" s="10"/>
+      <c r="U44" s="10"/>
+      <c r="V44" s="10"/>
+      <c r="W44" s="10"/>
+      <c r="X44" s="10"/>
+      <c r="Y44" s="10"/>
+      <c r="Z44" s="11"/>
     </row>
     <row r="45" spans="1:26">
       <c r="A45">
@@ -2276,22 +2276,22 @@
       <c r="J45">
         <v>14</v>
       </c>
-      <c r="K45" s="25"/>
-      <c r="L45" s="23"/>
-      <c r="M45" s="23"/>
-      <c r="N45" s="23"/>
-      <c r="O45" s="23"/>
-      <c r="P45" s="23"/>
-      <c r="Q45" s="23"/>
-      <c r="R45" s="40"/>
-      <c r="S45" s="25"/>
-      <c r="T45" s="23"/>
-      <c r="U45" s="23"/>
-      <c r="V45" s="23"/>
-      <c r="W45" s="23"/>
-      <c r="X45" s="23"/>
-      <c r="Y45" s="23"/>
-      <c r="Z45" s="24"/>
+      <c r="K45" s="12"/>
+      <c r="L45" s="10"/>
+      <c r="M45" s="10"/>
+      <c r="N45" s="10"/>
+      <c r="O45" s="10"/>
+      <c r="P45" s="10"/>
+      <c r="Q45" s="10"/>
+      <c r="R45" s="19"/>
+      <c r="S45" s="12"/>
+      <c r="T45" s="10"/>
+      <c r="U45" s="10"/>
+      <c r="V45" s="10"/>
+      <c r="W45" s="10"/>
+      <c r="X45" s="10"/>
+      <c r="Y45" s="10"/>
+      <c r="Z45" s="11"/>
     </row>
     <row r="46" spans="1:26">
       <c r="A46">
@@ -2322,22 +2322,22 @@
       <c r="J46">
         <v>15</v>
       </c>
-      <c r="K46" s="25"/>
-      <c r="L46" s="23"/>
-      <c r="M46" s="23"/>
-      <c r="N46" s="23"/>
-      <c r="O46" s="23"/>
-      <c r="P46" s="23"/>
-      <c r="Q46" s="23"/>
-      <c r="R46" s="40"/>
-      <c r="S46" s="25"/>
-      <c r="T46" s="23"/>
-      <c r="U46" s="23"/>
-      <c r="V46" s="23"/>
-      <c r="W46" s="23"/>
-      <c r="X46" s="23"/>
-      <c r="Y46" s="23"/>
-      <c r="Z46" s="24"/>
+      <c r="K46" s="12"/>
+      <c r="L46" s="10"/>
+      <c r="M46" s="10"/>
+      <c r="N46" s="10"/>
+      <c r="O46" s="10"/>
+      <c r="P46" s="10"/>
+      <c r="Q46" s="10"/>
+      <c r="R46" s="19"/>
+      <c r="S46" s="12"/>
+      <c r="T46" s="10"/>
+      <c r="U46" s="10"/>
+      <c r="V46" s="10"/>
+      <c r="W46" s="10"/>
+      <c r="X46" s="10"/>
+      <c r="Y46" s="10"/>
+      <c r="Z46" s="11"/>
     </row>
     <row r="47" spans="1:26">
       <c r="A47">
@@ -2364,22 +2364,22 @@
       <c r="J47">
         <v>16</v>
       </c>
-      <c r="K47" s="25"/>
-      <c r="L47" s="23"/>
-      <c r="M47" s="23"/>
-      <c r="N47" s="23"/>
-      <c r="O47" s="23"/>
-      <c r="P47" s="23"/>
-      <c r="Q47" s="23"/>
-      <c r="R47" s="40"/>
-      <c r="S47" s="25"/>
-      <c r="T47" s="23"/>
-      <c r="U47" s="23"/>
-      <c r="V47" s="23"/>
-      <c r="W47" s="23"/>
-      <c r="X47" s="23"/>
-      <c r="Y47" s="23"/>
-      <c r="Z47" s="24"/>
+      <c r="K47" s="12"/>
+      <c r="L47" s="10"/>
+      <c r="M47" s="10"/>
+      <c r="N47" s="10"/>
+      <c r="O47" s="10"/>
+      <c r="P47" s="10"/>
+      <c r="Q47" s="10"/>
+      <c r="R47" s="19"/>
+      <c r="S47" s="12"/>
+      <c r="T47" s="10"/>
+      <c r="U47" s="10"/>
+      <c r="V47" s="10"/>
+      <c r="W47" s="10"/>
+      <c r="X47" s="10"/>
+      <c r="Y47" s="10"/>
+      <c r="Z47" s="11"/>
     </row>
     <row r="48" spans="1:26" ht="15.75" thickBot="1">
       <c r="A48">
@@ -2406,66 +2406,66 @@
       <c r="J48">
         <v>17</v>
       </c>
-      <c r="K48" s="34"/>
-      <c r="L48" s="35"/>
-      <c r="M48" s="35"/>
-      <c r="N48" s="35"/>
-      <c r="O48" s="35"/>
-      <c r="P48" s="35"/>
-      <c r="Q48" s="35"/>
-      <c r="R48" s="41"/>
-      <c r="S48" s="34"/>
-      <c r="T48" s="35"/>
-      <c r="U48" s="35"/>
-      <c r="V48" s="35"/>
-      <c r="W48" s="35"/>
-      <c r="X48" s="35"/>
-      <c r="Y48" s="35"/>
-      <c r="Z48" s="36"/>
+      <c r="K48" s="13"/>
+      <c r="L48" s="14"/>
+      <c r="M48" s="14"/>
+      <c r="N48" s="14"/>
+      <c r="O48" s="14"/>
+      <c r="P48" s="14"/>
+      <c r="Q48" s="14"/>
+      <c r="R48" s="20"/>
+      <c r="S48" s="13"/>
+      <c r="T48" s="14"/>
+      <c r="U48" s="14"/>
+      <c r="V48" s="14"/>
+      <c r="W48" s="14"/>
+      <c r="X48" s="14"/>
+      <c r="Y48" s="14"/>
+      <c r="Z48" s="15"/>
     </row>
     <row r="49" spans="5:26" ht="15.75" thickTop="1">
       <c r="F49" s="5"/>
       <c r="G49" s="5"/>
-      <c r="K49" s="11" t="s">
+      <c r="K49" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="L49" s="11"/>
-      <c r="M49" s="11"/>
-      <c r="N49" s="11"/>
-      <c r="O49" s="11"/>
-      <c r="P49" s="11"/>
-      <c r="Q49" s="11"/>
-      <c r="R49" s="11"/>
-      <c r="S49" s="11" t="s">
+      <c r="L49" s="39"/>
+      <c r="M49" s="39"/>
+      <c r="N49" s="39"/>
+      <c r="O49" s="39"/>
+      <c r="P49" s="39"/>
+      <c r="Q49" s="39"/>
+      <c r="R49" s="39"/>
+      <c r="S49" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="T49" s="11"/>
-      <c r="U49" s="11"/>
-      <c r="V49" s="11"/>
-      <c r="W49" s="11"/>
-      <c r="X49" s="11"/>
-      <c r="Y49" s="11"/>
-      <c r="Z49" s="11"/>
+      <c r="T49" s="39"/>
+      <c r="U49" s="39"/>
+      <c r="V49" s="39"/>
+      <c r="W49" s="39"/>
+      <c r="X49" s="39"/>
+      <c r="Y49" s="39"/>
+      <c r="Z49" s="39"/>
     </row>
     <row r="50" spans="5:26">
-      <c r="E50" s="7"/>
-      <c r="F50" s="8"/>
-      <c r="G50" s="8"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="41"/>
+      <c r="G50" s="41"/>
     </row>
     <row r="51" spans="5:26">
-      <c r="E51" s="7"/>
-      <c r="F51" s="8"/>
-      <c r="G51" s="8"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="41"/>
+      <c r="G51" s="41"/>
     </row>
     <row r="52" spans="5:26">
-      <c r="E52" s="7"/>
-      <c r="F52" s="8"/>
-      <c r="G52" s="8"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="41"/>
+      <c r="G52" s="41"/>
     </row>
     <row r="53" spans="5:26">
-      <c r="E53" s="7"/>
-      <c r="F53" s="9"/>
-      <c r="G53" s="9"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="21"/>
+      <c r="G53" s="21"/>
     </row>
     <row r="54" spans="5:26">
       <c r="E54" s="5"/>
@@ -3469,6 +3469,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="F52:G52"/>
     <mergeCell ref="F53:G53"/>
     <mergeCell ref="K32:R32"/>
     <mergeCell ref="S32:Z32"/>
@@ -3483,11 +3488,6 @@
     <mergeCell ref="N35:O36"/>
     <mergeCell ref="K49:R49"/>
     <mergeCell ref="S49:Z49"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="F52:G52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>